<commit_message>
Add base oficial intento 1
</commit_message>
<xml_diff>
--- a/Componentes.xlsx
+++ b/Componentes.xlsx
@@ -1,69 +1,140 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1567651d2153b5b6/Documentos/Universidad/7_semestre/Proyecto_IRB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_AD4D2F04E46CFB4ACB3E201B6D10DE6E683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CD9B77C-4980-473F-A499-2147374A8E2C}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="11_AD4D2F04E46CFB4ACB3E201B6D10DE6E683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7DD7D07-78E9-41F0-A7E9-F6E9E0231F16}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>Función</t>
+  </si>
+  <si>
+    <t>Conecciones necesarias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medidas 3D en mm. </t>
+  </si>
+  <si>
+    <t>Voltaje necesario</t>
+  </si>
+  <si>
+    <t>Precio total</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
   <si>
     <t>Batería de Litio</t>
   </si>
   <si>
-    <t>Función</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>Conecciones necesarias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medidas 3D en mm. </t>
-  </si>
-  <si>
-    <t>Voltaje necesario</t>
-  </si>
-  <si>
-    <t>Precio total</t>
-  </si>
-  <si>
-    <t>Observaciones</t>
+    <t>Fuente de poder</t>
+  </si>
+  <si>
+    <t>(??)</t>
   </si>
   <si>
     <t xml:space="preserve">Rasberi pi pico </t>
   </si>
   <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
-    <t>UPS</t>
+    <t>Micro usb para la fuente de 
+poder y pines para I/O</t>
+  </si>
+  <si>
+    <t>Alimentada por USB o por una
+ fuente externa de 1.8V a 5.5V</t>
   </si>
   <si>
     <t>Mlni-360</t>
   </si>
   <si>
+    <t>IN: Positivo (VIN) y GND
+OUT: Positivo VOUT y GND</t>
+  </si>
+  <si>
+    <t>17 x 11 x 3.8</t>
+  </si>
+  <si>
+    <t>4.75 V - 23 V</t>
+  </si>
+  <si>
+    <t>TB6612FNG</t>
+  </si>
+  <si>
+    <t>Puente H</t>
+  </si>
+  <si>
+    <t>https://c2plabs.com/blog/2021/09/12/controlling-dc-motor-using-raspberry-pi-pico-rp2040-and-tb6612fng/</t>
+  </si>
+  <si>
+    <t>20 x 20</t>
+  </si>
+  <si>
+    <t>2.7 V - 5V</t>
+  </si>
+  <si>
+    <t>reduce-enc-motors</t>
+  </si>
+  <si>
     <t>Conectores</t>
+  </si>
+  <si>
+    <t>Pernos y tuercas</t>
+  </si>
+  <si>
+    <t>Ruedas tipo B</t>
+  </si>
+  <si>
+    <t>Rueda universal</t>
+  </si>
+  <si>
+    <t>Placa</t>
+  </si>
+  <si>
+    <t>Reductor voltaje</t>
+  </si>
+  <si>
+    <t>Motor Solenoide</t>
+  </si>
+  <si>
+    <t>Correa</t>
+  </si>
+  <si>
+    <t>Correa Cerrada 6 Mm Gt2 Largo 110 Mm Pack 3 Unidades Cnc | Cuotas sin interés</t>
   </si>
 </sst>
 </file>
@@ -79,10 +150,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,15 +175,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -124,6 +204,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87AB6E1C-97C7-F390-14F6-231B0A348048}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15249525" y="1933575"/>
+          <a:ext cx="4572000" cy="1666875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,78 +522,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:K9"/>
+  <dimension ref="C3:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="19.46484375" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" customWidth="1"/>
+    <col min="4" max="4" width="71.06640625" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="25.3984375" customWidth="1"/>
-    <col min="7" max="7" width="19.265625" customWidth="1"/>
-    <col min="8" max="8" width="19.1328125" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="26.73046875" customWidth="1"/>
     <col min="9" max="9" width="13.59765625" customWidth="1"/>
     <col min="10" max="10" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+    </row>
+    <row r="4" spans="3:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C9" s="2"/>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{E3B44F15-36E3-4533-8D17-4EA5F6B27605}"/>
+    <hyperlink ref="D10" r:id="rId2" location="polycard_client=search-nordic&amp;position=16&amp;search_layout=stack&amp;type=item&amp;tracking_id=5dd93bf1-7bf9-4107-aaf6-b869dcf0d766" display="https://articulo.mercadolibre.cl/MLC-540015747-correa-cerrada-6-mm-gt2-largo-110-mm-pack-3-unidades-cnc-_JM - polycard_client=search-nordic&amp;position=16&amp;search_layout=stack&amp;type=item&amp;tracking_id=5dd93bf1-7bf9-4107-aaf6-b869dcf0d766" xr:uid="{09C6475A-04EF-4A6C-BDB0-088FDC8B0D87}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>